<commit_message>
Script for creating gantt timeline
</commit_message>
<xml_diff>
--- a/Gantt/data/gantt_timeline_abroad.xlsx
+++ b/Gantt/data/gantt_timeline_abroad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\python\scripts\Gantt\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57280C3D-4BA6-4EA5-9D3E-76858670E7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3233785-4F04-40AF-A89B-4AEC5CBA3CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{B293A86B-E8B9-4C93-8730-62896337CEB7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Design graph data</t>
   </si>
@@ -45,9 +45,6 @@
     <t>End</t>
   </si>
   <si>
-    <t>Implement Multi-vehicle routing solver for GT</t>
-  </si>
-  <si>
     <t>Duration (optional)</t>
   </si>
   <si>
@@ -58,6 +55,19 @@
   </si>
   <si>
     <t>Return</t>
+  </si>
+  <si>
+    <t>Implement Multi-vehicle
+routing solver for GT</t>
+  </si>
+  <si>
+    <t>Focus on writing</t>
+  </si>
+  <si>
+    <t>Extend the simulation env.</t>
+  </si>
+  <si>
+    <t>Design and train GNN</t>
   </si>
 </sst>
 </file>
@@ -132,7 +142,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1"/>
@@ -142,6 +152,10 @@
     <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
@@ -459,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF9B430-0097-4B95-886E-4F7DB8DD73AF}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,11 +485,12 @@
     <col min="2" max="2" width="30.5703125" customWidth="1"/>
     <col min="3" max="3" width="40.5703125" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -484,18 +499,18 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4">
-        <v>44819</v>
+        <v>44805</v>
       </c>
       <c r="C2" s="4">
-        <v>44820</v>
+        <v>44806</v>
       </c>
       <c r="D2" s="3">
         <f>C2-B2</f>
@@ -507,43 +522,88 @@
         <v>0</v>
       </c>
       <c r="B3" s="6">
-        <v>44819</v>
+        <v>44805</v>
       </c>
       <c r="C3" s="6">
         <v>44895</v>
       </c>
       <c r="D3" s="5">
-        <f t="shared" ref="D3:D15" si="0">C3-B3</f>
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
+        <f t="shared" ref="D3:D9" si="0">C3-B3</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="B4" s="4">
+        <v>44835</v>
+      </c>
+      <c r="C4" s="4">
         <v>44866</v>
-      </c>
-      <c r="C4" s="4">
-        <v>44937</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="6">
-        <v>44984</v>
-      </c>
-      <c r="C5" s="6">
-        <v>44985</v>
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="10">
+        <v>44896</v>
+      </c>
+      <c r="C5" s="10">
+        <v>44972</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="10">
+        <v>44927</v>
+      </c>
+      <c r="C6" s="10">
+        <v>44985</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="10">
+        <v>44819</v>
+      </c>
+      <c r="C7" s="10">
+        <v>44895</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6">
+        <v>44984</v>
+      </c>
+      <c r="C8" s="6">
+        <v>44985</v>
+      </c>
+      <c r="D8" s="3">
+        <f>C8-B8</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>